<commit_message>
state prefix space fix
</commit_message>
<xml_diff>
--- a/input/StockList.xlsx
+++ b/input/StockList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B88CA72-AF84-C64B-9F48-9629F1BDD27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D4CADF-60CD-FB4D-98E5-3A60E522EC2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,17 +13,246 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Symbol</t>
   </si>
   <si>
     <t>BBCA</t>
+  </si>
+  <si>
+    <t>BBRI</t>
+  </si>
+  <si>
+    <t>TLKM</t>
+  </si>
+  <si>
+    <t>ASII</t>
+  </si>
+  <si>
+    <t>BMRI</t>
+  </si>
+  <si>
+    <t>UNVR</t>
+  </si>
+  <si>
+    <t>CPIN</t>
+  </si>
+  <si>
+    <t>BBNI</t>
+  </si>
+  <si>
+    <t>KLBF</t>
+  </si>
+  <si>
+    <t>INDF</t>
+  </si>
+  <si>
+    <t>SMGR</t>
+  </si>
+  <si>
+    <t>INKP</t>
+  </si>
+  <si>
+    <t>BRPT</t>
+  </si>
+  <si>
+    <t>GGRM</t>
+  </si>
+  <si>
+    <t>ICBP</t>
+  </si>
+  <si>
+    <t>INTP</t>
+  </si>
+  <si>
+    <t>ADRO</t>
+  </si>
+  <si>
+    <t>HMSP</t>
+  </si>
+  <si>
+    <t>PGAS</t>
+  </si>
+  <si>
+    <t>TBIG</t>
+  </si>
+  <si>
+    <t>ACES</t>
+  </si>
+  <si>
+    <t>UNTR</t>
+  </si>
+  <si>
+    <t>TKIM</t>
+  </si>
+  <si>
+    <t>EXCL</t>
+  </si>
+  <si>
+    <t>JSMR</t>
+  </si>
+  <si>
+    <t>BTPS</t>
+  </si>
+  <si>
+    <t>SCMA</t>
+  </si>
+  <si>
+    <t>BBTN</t>
+  </si>
+  <si>
+    <t>CTRA</t>
+  </si>
+  <si>
+    <t>PTBA</t>
+  </si>
+  <si>
+    <t>ANTM</t>
+  </si>
+  <si>
+    <t>PWON</t>
+  </si>
+  <si>
+    <t>SMRA</t>
+  </si>
+  <si>
+    <t>MAPI</t>
+  </si>
+  <si>
+    <t>MNCN</t>
+  </si>
+  <si>
+    <t>LPKR</t>
+  </si>
+  <si>
+    <t>BSDE</t>
+  </si>
+  <si>
+    <t>AKRA</t>
+  </si>
+  <si>
+    <t>JPFA</t>
+  </si>
+  <si>
+    <t>SIDO</t>
+  </si>
+  <si>
+    <t>ISAT</t>
+  </si>
+  <si>
+    <t>APIC</t>
+  </si>
+  <si>
+    <t>WIKA</t>
+  </si>
+  <si>
+    <t>PTPP</t>
+  </si>
+  <si>
+    <t>BOGA</t>
+  </si>
+  <si>
+    <t>DMAS</t>
+  </si>
+  <si>
+    <t>ERAA</t>
+  </si>
+  <si>
+    <t>ITMG</t>
+  </si>
+  <si>
+    <t>WSKT</t>
+  </si>
+  <si>
+    <t>MEDC</t>
+  </si>
+  <si>
+    <t>PNLF</t>
+  </si>
+  <si>
+    <t>LPPF</t>
+  </si>
+  <si>
+    <t>SSMS</t>
+  </si>
+  <si>
+    <t>SMSM</t>
+  </si>
+  <si>
+    <t>BUMI</t>
+  </si>
+  <si>
+    <t>BJBR</t>
+  </si>
+  <si>
+    <t>MYRX</t>
+  </si>
+  <si>
+    <t>BJTM</t>
+  </si>
+  <si>
+    <t>WSBP</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>RALS</t>
+  </si>
+  <si>
+    <t>LSIP</t>
+  </si>
+  <si>
+    <t>IIKP</t>
+  </si>
+  <si>
+    <t>TRAM</t>
+  </si>
+  <si>
+    <t>NATO</t>
+  </si>
+  <si>
+    <t>TAMU</t>
+  </si>
+  <si>
+    <t>AALI</t>
+  </si>
+  <si>
+    <t>RIMO</t>
+  </si>
+  <si>
+    <t>TARA</t>
+  </si>
+  <si>
+    <t>BLTA</t>
+  </si>
+  <si>
+    <t>POOL</t>
+  </si>
+  <si>
+    <t>SIAP</t>
+  </si>
+  <si>
+    <t>SUGI</t>
+  </si>
+  <si>
+    <t>INVS</t>
   </si>
 </sst>
 </file>
@@ -408,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -429,6 +658,371 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>